<commit_message>
added results of 128
</commit_message>
<xml_diff>
--- a/Assignment3/results.xlsx
+++ b/Assignment3/results.xlsx
@@ -13,17 +13,20 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1589209359" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1589209359" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1589209359"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1589209359"/>
+      <pm:revision xmlns:pm="smNativeData" day="1589279881" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1589279881" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1589279881" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1589279881"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Seq</t>
+  </si>
   <si>
     <t>linear</t>
   </si>
@@ -66,7 +69,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1589209359" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1589279881" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -81,7 +84,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1589209359" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1589279881" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -103,7 +106,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1589209359" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1589279881" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -125,7 +128,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1589209359"/>
+          <pm:border xmlns:pm="smNativeData" id="1589279881"/>
         </ext>
       </extLst>
     </border>
@@ -144,7 +147,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1589209359"/>
+          <pm:border xmlns:pm="smNativeData" id="1589279881"/>
         </ext>
       </extLst>
     </border>
@@ -162,7 +165,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1589209359" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1589279881" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -426,17 +429,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F64"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="H14" sqref="H13:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2"/>
     </row>
@@ -447,6 +455,9 @@
       <c r="B3" t="n">
         <v>3.31199999999999983</v>
       </c>
+      <c r="C3" t="n">
+        <v>4.21199999999999974</v>
+      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
@@ -456,6 +467,9 @@
       <c r="B4" t="n">
         <v>1.98300000000000018</v>
       </c>
+      <c r="C4" t="n">
+        <v>2.30699999999999994</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
@@ -465,6 +479,9 @@
       <c r="B5" t="n">
         <v>0.958999999999999986</v>
       </c>
+      <c r="C5" t="n">
+        <v>1.33400000000000007</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
@@ -474,6 +491,9 @@
       <c r="B6" t="n">
         <v>0.951999999999999957</v>
       </c>
+      <c r="C6" t="n">
+        <v>0.672000000000000064</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
@@ -481,7 +501,10 @@
         <v>128</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.653000000000000025</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.653000000000000025</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -493,7 +516,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -504,6 +527,9 @@
       <c r="B11" t="n">
         <v>3.35199999999999987</v>
       </c>
+      <c r="C11" t="n">
+        <v>4.23500000000000032</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
@@ -513,6 +539,9 @@
       <c r="B12" t="n">
         <v>1.95899999999999999</v>
       </c>
+      <c r="C12" t="n">
+        <v>2.30100000000000016</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
@@ -522,6 +551,9 @@
       <c r="B13" t="n">
         <v>0.965000000000000036</v>
       </c>
+      <c r="C13" t="n">
+        <v>1.31299999999999994</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
@@ -531,14 +563,26 @@
       <c r="B14" t="n">
         <v>0.944999999999999929</v>
       </c>
+      <c r="C14" t="n">
+        <v>0.672000000000000064</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="5:5">
+    <row r="15" spans="1:5">
+      <c r="A15" t="n">
+        <v>128</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.655000000000000071</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.655000000000000071</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -549,6 +593,9 @@
       <c r="B17" t="n">
         <v>3.40200000000000014</v>
       </c>
+      <c r="C17" t="n">
+        <v>4.21600000000000019</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
@@ -558,6 +605,9 @@
       <c r="B18" t="n">
         <v>1.96700000000000017</v>
       </c>
+      <c r="C18" t="n">
+        <v>2.28900000000000015</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
@@ -567,6 +617,9 @@
       <c r="B19" t="n">
         <v>0.967999999999999972</v>
       </c>
+      <c r="C19" t="n">
+        <v>1.31000000000000005</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
@@ -576,14 +629,26 @@
       <c r="B20" t="n">
         <v>0.950999999999999979</v>
       </c>
+      <c r="C20" t="n">
+        <v>0.687999999999999901</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="5:5">
+    <row r="21" spans="1:5">
+      <c r="A21" t="n">
+        <v>128</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.663000000000000078</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.663000000000000078</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -594,6 +659,9 @@
       <c r="B23" t="n">
         <v>3.32699999999999996</v>
       </c>
+      <c r="C23" t="n">
+        <v>4.20899999999999963</v>
+      </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
@@ -603,6 +671,9 @@
       <c r="B24" t="n">
         <v>1.97400000000000002</v>
       </c>
+      <c r="C24" t="n">
+        <v>2.2589999999999999</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
@@ -612,6 +683,9 @@
       <c r="B25" t="n">
         <v>0.976999999999999957</v>
       </c>
+      <c r="C25" t="n">
+        <v>1.33200000000000007</v>
+      </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
@@ -621,14 +695,26 @@
       <c r="B26" t="n">
         <v>0.958999999999999986</v>
       </c>
+      <c r="C26" t="n">
+        <v>0.671000000000000085</v>
+      </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="5:5">
+    <row r="27" spans="1:5">
+      <c r="A27" t="n">
+        <v>128</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.645000000000000018</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.645000000000000018</v>
+      </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -639,6 +725,9 @@
       <c r="B29" t="n">
         <v>3.39999999999999991</v>
       </c>
+      <c r="C29" t="n">
+        <v>4.2240000000000002</v>
+      </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5">
@@ -648,66 +737,109 @@
       <c r="B30" t="n">
         <v>1.97100000000000009</v>
       </c>
+      <c r="C30" t="n">
+        <v>2.24500000000000011</v>
+      </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:3">
       <c r="A31" t="n">
         <v>32</v>
       </c>
       <c r="B31" t="n">
         <v>0.974000000000000021</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="n">
+        <v>1.27699999999999991</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="n">
         <v>64</v>
       </c>
       <c r="B32" t="n">
         <v>0.95</v>
       </c>
+      <c r="C32" t="n">
+        <v>0.672000000000000064</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="n">
+        <v>128</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.662000000000000011</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.662000000000000011</v>
+      </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="n">
         <v>8</v>
       </c>
       <c r="B35" t="n">
         <v>3.36399999999999988</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="n">
+        <v>4.24600000000000044</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="n">
         <v>16</v>
       </c>
       <c r="B36" t="n">
         <v>1.91799999999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="C36" t="n">
+        <v>2.30600000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="n">
         <v>32</v>
       </c>
       <c r="B37" t="n">
         <v>0.978999999999999915</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="C37" t="n">
+        <v>1.29800000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="n">
         <v>64</v>
       </c>
       <c r="B38" t="n">
         <v>1.05899999999999994</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.679000000000000092</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="n">
+        <v>128</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.761000000000000032</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.761000000000000032</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1589209359" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1589279881" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -716,14 +848,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1589209359" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1589209359" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1589279881" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1589279881" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1589209359" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1589279881" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>